<commit_message>
Remove build and cache folders
</commit_message>
<xml_diff>
--- a/Evaluation_Result.xlsx
+++ b/Evaluation_Result.xlsx
@@ -588,7 +588,7 @@
         <v>user2</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1">
         <v>2</v>
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1">
         <v>2</v>

</xml_diff>